<commit_message>
update with gender of student
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="460">
   <si>
     <t>goc_no</t>
   </si>
@@ -1395,6 +1395,15 @@
   </si>
   <si>
     <t>TVL - HE</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -1769,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,6 +1818,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1838,8 +1850,8 @@
       <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="J2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1870,8 +1882,8 @@
       <c r="I3" t="s">
         <v>89</v>
       </c>
-      <c r="J3">
-        <v>2</v>
+      <c r="J3" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1902,8 +1914,8 @@
       <c r="I4" t="s">
         <v>89</v>
       </c>
-      <c r="J4">
-        <v>3</v>
+      <c r="J4" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1934,8 +1946,8 @@
       <c r="I5" t="s">
         <v>89</v>
       </c>
-      <c r="J5">
-        <v>4</v>
+      <c r="J5" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1966,8 +1978,8 @@
       <c r="I6" t="s">
         <v>89</v>
       </c>
-      <c r="J6">
-        <v>5</v>
+      <c r="J6" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1998,8 +2010,8 @@
       <c r="I7" t="s">
         <v>89</v>
       </c>
-      <c r="J7">
-        <v>6</v>
+      <c r="J7" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2030,8 +2042,8 @@
       <c r="I8" t="s">
         <v>89</v>
       </c>
-      <c r="J8">
-        <v>7</v>
+      <c r="J8" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2062,8 +2074,8 @@
       <c r="I9" t="s">
         <v>89</v>
       </c>
-      <c r="J9">
-        <v>8</v>
+      <c r="J9" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2094,8 +2106,8 @@
       <c r="I10" t="s">
         <v>89</v>
       </c>
-      <c r="J10">
-        <v>9</v>
+      <c r="J10" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2126,8 +2138,8 @@
       <c r="I11" t="s">
         <v>89</v>
       </c>
-      <c r="J11">
-        <v>10</v>
+      <c r="J11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2158,8 +2170,8 @@
       <c r="I12" t="s">
         <v>89</v>
       </c>
-      <c r="J12">
-        <v>11</v>
+      <c r="J12" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2188,8 +2200,8 @@
       <c r="I13" t="s">
         <v>89</v>
       </c>
-      <c r="J13">
-        <v>12</v>
+      <c r="J13" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2220,8 +2232,8 @@
       <c r="I14" t="s">
         <v>89</v>
       </c>
-      <c r="J14">
-        <v>13</v>
+      <c r="J14" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2252,8 +2264,8 @@
       <c r="I15" t="s">
         <v>89</v>
       </c>
-      <c r="J15">
-        <v>14</v>
+      <c r="J15" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2284,8 +2296,8 @@
       <c r="I16" t="s">
         <v>89</v>
       </c>
-      <c r="J16">
-        <v>15</v>
+      <c r="J16" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2316,8 +2328,8 @@
       <c r="I17" t="s">
         <v>89</v>
       </c>
-      <c r="J17">
-        <v>16</v>
+      <c r="J17" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2348,8 +2360,8 @@
       <c r="I18" t="s">
         <v>89</v>
       </c>
-      <c r="J18">
-        <v>17</v>
+      <c r="J18" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2380,8 +2392,8 @@
       <c r="I19" t="s">
         <v>89</v>
       </c>
-      <c r="J19">
-        <v>18</v>
+      <c r="J19" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2412,8 +2424,8 @@
       <c r="I20" t="s">
         <v>89</v>
       </c>
-      <c r="J20">
-        <v>19</v>
+      <c r="J20" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2444,8 +2456,8 @@
       <c r="I21" t="s">
         <v>89</v>
       </c>
-      <c r="J21">
-        <v>20</v>
+      <c r="J21" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2476,8 +2488,8 @@
       <c r="I22" t="s">
         <v>89</v>
       </c>
-      <c r="J22">
-        <v>21</v>
+      <c r="J22" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2508,8 +2520,8 @@
       <c r="I23" t="s">
         <v>89</v>
       </c>
-      <c r="J23">
-        <v>22</v>
+      <c r="J23" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2540,8 +2552,8 @@
       <c r="I24" t="s">
         <v>89</v>
       </c>
-      <c r="J24">
-        <v>23</v>
+      <c r="J24" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2572,8 +2584,8 @@
       <c r="I25" t="s">
         <v>89</v>
       </c>
-      <c r="J25">
-        <v>24</v>
+      <c r="J25" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2604,8 +2616,8 @@
       <c r="I26" t="s">
         <v>89</v>
       </c>
-      <c r="J26">
-        <v>25</v>
+      <c r="J26" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2636,8 +2648,8 @@
       <c r="I27" t="s">
         <v>89</v>
       </c>
-      <c r="J27">
-        <v>26</v>
+      <c r="J27" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2668,8 +2680,8 @@
       <c r="I28" t="s">
         <v>89</v>
       </c>
-      <c r="J28">
-        <v>27</v>
+      <c r="J28" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2700,8 +2712,8 @@
       <c r="I29" t="s">
         <v>89</v>
       </c>
-      <c r="J29">
-        <v>28</v>
+      <c r="J29" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2732,8 +2744,8 @@
       <c r="I30" t="s">
         <v>89</v>
       </c>
-      <c r="J30">
-        <v>29</v>
+      <c r="J30" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2764,8 +2776,8 @@
       <c r="I31" t="s">
         <v>89</v>
       </c>
-      <c r="J31">
-        <v>30</v>
+      <c r="J31" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2796,8 +2808,8 @@
       <c r="I32" t="s">
         <v>89</v>
       </c>
-      <c r="J32">
-        <v>31</v>
+      <c r="J32" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2828,8 +2840,8 @@
       <c r="I33" t="s">
         <v>89</v>
       </c>
-      <c r="J33">
-        <v>32</v>
+      <c r="J33" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2860,8 +2872,8 @@
       <c r="I34" t="s">
         <v>89</v>
       </c>
-      <c r="J34">
-        <v>33</v>
+      <c r="J34" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2892,8 +2904,8 @@
       <c r="I35" t="s">
         <v>89</v>
       </c>
-      <c r="J35">
-        <v>34</v>
+      <c r="J35" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2924,8 +2936,8 @@
       <c r="I36" t="s">
         <v>89</v>
       </c>
-      <c r="J36">
-        <v>35</v>
+      <c r="J36" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2954,8 +2966,8 @@
       <c r="I37" t="s">
         <v>89</v>
       </c>
-      <c r="J37">
-        <v>36</v>
+      <c r="J37" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2984,8 +2996,8 @@
       <c r="I38" t="s">
         <v>89</v>
       </c>
-      <c r="J38">
-        <v>37</v>
+      <c r="J38" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3016,8 +3028,8 @@
       <c r="I39" t="s">
         <v>89</v>
       </c>
-      <c r="J39">
-        <v>38</v>
+      <c r="J39" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3048,8 +3060,8 @@
       <c r="I40" t="s">
         <v>89</v>
       </c>
-      <c r="J40">
-        <v>39</v>
+      <c r="J40" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3080,8 +3092,8 @@
       <c r="I41" t="s">
         <v>89</v>
       </c>
-      <c r="J41">
-        <v>40</v>
+      <c r="J41" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3112,8 +3124,8 @@
       <c r="I42" t="s">
         <v>89</v>
       </c>
-      <c r="J42">
-        <v>41</v>
+      <c r="J42" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3144,8 +3156,8 @@
       <c r="I43" t="s">
         <v>89</v>
       </c>
-      <c r="J43">
-        <v>42</v>
+      <c r="J43" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3176,8 +3188,8 @@
       <c r="I44" t="s">
         <v>89</v>
       </c>
-      <c r="J44">
-        <v>43</v>
+      <c r="J44" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3208,8 +3220,8 @@
       <c r="I45" t="s">
         <v>89</v>
       </c>
-      <c r="J45">
-        <v>44</v>
+      <c r="J45" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3240,8 +3252,8 @@
       <c r="I46" t="s">
         <v>89</v>
       </c>
-      <c r="J46">
-        <v>45</v>
+      <c r="J46" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3272,6 +3284,9 @@
       <c r="I47" t="s">
         <v>89</v>
       </c>
+      <c r="J47" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3301,8 +3316,11 @@
       <c r="I48" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>383</v>
       </c>
@@ -3330,8 +3348,11 @@
       <c r="I49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>384</v>
       </c>
@@ -3359,8 +3380,11 @@
       <c r="I50" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>385</v>
       </c>
@@ -3388,8 +3412,11 @@
       <c r="I51" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>386</v>
       </c>
@@ -3417,8 +3444,11 @@
       <c r="I52" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -3446,8 +3476,11 @@
       <c r="I53" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>388</v>
       </c>
@@ -3475,8 +3508,11 @@
       <c r="I54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>389</v>
       </c>
@@ -3504,8 +3540,11 @@
       <c r="I55" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>390</v>
       </c>
@@ -3533,8 +3572,11 @@
       <c r="I56" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>391</v>
       </c>
@@ -3562,8 +3604,11 @@
       <c r="I57" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>392</v>
       </c>
@@ -3591,8 +3636,11 @@
       <c r="I58" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>393</v>
       </c>
@@ -3620,8 +3668,11 @@
       <c r="I59" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>394</v>
       </c>
@@ -3649,8 +3700,11 @@
       <c r="I60" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>395</v>
       </c>
@@ -3678,8 +3732,11 @@
       <c r="I61" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>396</v>
       </c>
@@ -3707,8 +3764,11 @@
       <c r="I62" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>397</v>
       </c>
@@ -3736,8 +3796,11 @@
       <c r="I63" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>398</v>
       </c>
@@ -3765,8 +3828,11 @@
       <c r="I64" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>399</v>
       </c>
@@ -3794,8 +3860,11 @@
       <c r="I65" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>400</v>
       </c>
@@ -3823,8 +3892,11 @@
       <c r="I66" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>401</v>
       </c>
@@ -3852,8 +3924,11 @@
       <c r="I67" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>402</v>
       </c>
@@ -3881,8 +3956,11 @@
       <c r="I68" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>403</v>
       </c>
@@ -3910,8 +3988,11 @@
       <c r="I69" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>404</v>
       </c>
@@ -3939,8 +4020,11 @@
       <c r="I70" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>405</v>
       </c>
@@ -3968,8 +4052,11 @@
       <c r="I71" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>406</v>
       </c>
@@ -3997,8 +4084,11 @@
       <c r="I72" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>407</v>
       </c>
@@ -4026,8 +4116,11 @@
       <c r="I73" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>408</v>
       </c>
@@ -4055,8 +4148,11 @@
       <c r="I74" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -4084,8 +4180,11 @@
       <c r="I75" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>410</v>
       </c>
@@ -4113,8 +4212,11 @@
       <c r="I76" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>411</v>
       </c>
@@ -4142,8 +4244,11 @@
       <c r="I77" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>412</v>
       </c>
@@ -4171,8 +4276,11 @@
       <c r="I78" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>413</v>
       </c>
@@ -4200,8 +4308,11 @@
       <c r="I79" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>414</v>
       </c>
@@ -4229,8 +4340,11 @@
       <c r="I80" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>415</v>
       </c>
@@ -4258,8 +4372,11 @@
       <c r="I81" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>416</v>
       </c>
@@ -4287,8 +4404,11 @@
       <c r="I82" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>417</v>
       </c>
@@ -4316,8 +4436,11 @@
       <c r="I83" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>418</v>
       </c>
@@ -4345,8 +4468,11 @@
       <c r="I84" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>419</v>
       </c>
@@ -4374,8 +4500,11 @@
       <c r="I85" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>420</v>
       </c>
@@ -4400,8 +4529,11 @@
       <c r="I86" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>421</v>
       </c>
@@ -4429,8 +4561,11 @@
       <c r="I87" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>422</v>
       </c>
@@ -4458,8 +4593,11 @@
       <c r="I88" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>423</v>
       </c>
@@ -4487,8 +4625,11 @@
       <c r="I89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>424</v>
       </c>
@@ -4516,8 +4657,11 @@
       <c r="I90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>425</v>
       </c>
@@ -4545,8 +4689,11 @@
       <c r="I91" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>426</v>
       </c>
@@ -4574,8 +4721,11 @@
       <c r="I92" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>427</v>
       </c>
@@ -4603,8 +4753,11 @@
       <c r="I93" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>428</v>
       </c>
@@ -4632,8 +4785,11 @@
       <c r="I94" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>429</v>
       </c>
@@ -4661,8 +4817,11 @@
       <c r="I95" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>430</v>
       </c>
@@ -4690,8 +4849,11 @@
       <c r="I96" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>431</v>
       </c>
@@ -4719,8 +4881,11 @@
       <c r="I97" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>432</v>
       </c>
@@ -4748,8 +4913,11 @@
       <c r="I98" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>433</v>
       </c>
@@ -4777,8 +4945,11 @@
       <c r="I99" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>434</v>
       </c>
@@ -4806,8 +4977,11 @@
       <c r="I100" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>435</v>
       </c>
@@ -4835,8 +5009,11 @@
       <c r="I101" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>436</v>
       </c>
@@ -4864,8 +5041,11 @@
       <c r="I102" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>437</v>
       </c>
@@ -4893,8 +5073,11 @@
       <c r="I103" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>438</v>
       </c>
@@ -4922,8 +5105,11 @@
       <c r="I104" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>439</v>
       </c>
@@ -4951,8 +5137,11 @@
       <c r="I105" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>440</v>
       </c>
@@ -4980,8 +5169,11 @@
       <c r="I106" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>441</v>
       </c>
@@ -5009,8 +5201,11 @@
       <c r="I107" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>442</v>
       </c>
@@ -5038,8 +5233,11 @@
       <c r="I108" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>443</v>
       </c>
@@ -5067,8 +5265,11 @@
       <c r="I109" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>444</v>
       </c>
@@ -5096,8 +5297,11 @@
       <c r="I110" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>445</v>
       </c>
@@ -5125,8 +5329,11 @@
       <c r="I111" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>446</v>
       </c>
@@ -5154,8 +5361,11 @@
       <c r="I112" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>447</v>
       </c>
@@ -5183,8 +5393,11 @@
       <c r="I113" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>448</v>
       </c>
@@ -5212,8 +5425,11 @@
       <c r="I114" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>449</v>
       </c>
@@ -5241,8 +5457,11 @@
       <c r="I115" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>450</v>
       </c>
@@ -5270,8 +5489,11 @@
       <c r="I116" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>451</v>
       </c>
@@ -5299,8 +5521,11 @@
       <c r="I117" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>452</v>
       </c>
@@ -5328,8 +5553,11 @@
       <c r="I118" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>453</v>
       </c>
@@ -5357,8 +5585,11 @@
       <c r="I119" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>454</v>
       </c>
@@ -5385,6 +5616,9 @@
       </c>
       <c r="I120" t="s">
         <v>89</v>
+      </c>
+      <c r="J120" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Form for student regular and irregular
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="463">
   <si>
     <t>goc_no</t>
   </si>
@@ -1404,6 +1404,15 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>student_type</t>
+  </si>
+  <si>
+    <t>New Student</t>
+  </si>
+  <si>
+    <t>Transferee</t>
   </si>
 </sst>
 </file>
@@ -1776,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,9 +1797,10 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1821,8 +1831,11 @@
       <c r="J1" s="2" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>336</v>
       </c>
@@ -1853,8 +1866,11 @@
       <c r="J2" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>337</v>
       </c>
@@ -1885,8 +1901,11 @@
       <c r="J3" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>338</v>
       </c>
@@ -1917,8 +1936,11 @@
       <c r="J4" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>339</v>
       </c>
@@ -1949,8 +1971,11 @@
       <c r="J5" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>340</v>
       </c>
@@ -1981,8 +2006,11 @@
       <c r="J6" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>341</v>
       </c>
@@ -2013,8 +2041,11 @@
       <c r="J7" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>342</v>
       </c>
@@ -2045,8 +2076,11 @@
       <c r="J8" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>343</v>
       </c>
@@ -2077,8 +2111,11 @@
       <c r="J9" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>344</v>
       </c>
@@ -2109,8 +2146,11 @@
       <c r="J10" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>345</v>
       </c>
@@ -2141,8 +2181,11 @@
       <c r="J11" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>346</v>
       </c>
@@ -2173,8 +2216,11 @@
       <c r="J12" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>347</v>
       </c>
@@ -2203,8 +2249,11 @@
       <c r="J13" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>348</v>
       </c>
@@ -2235,8 +2284,11 @@
       <c r="J14" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>349</v>
       </c>
@@ -2267,8 +2319,11 @@
       <c r="J15" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>350</v>
       </c>
@@ -2299,8 +2354,11 @@
       <c r="J16" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>351</v>
       </c>
@@ -2331,8 +2389,11 @@
       <c r="J17" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>352</v>
       </c>
@@ -2363,8 +2424,11 @@
       <c r="J18" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>353</v>
       </c>
@@ -2395,8 +2459,11 @@
       <c r="J19" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>354</v>
       </c>
@@ -2427,8 +2494,11 @@
       <c r="J20" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>355</v>
       </c>
@@ -2459,8 +2529,11 @@
       <c r="J21" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>356</v>
       </c>
@@ -2491,8 +2564,11 @@
       <c r="J22" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>357</v>
       </c>
@@ -2523,8 +2599,11 @@
       <c r="J23" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>358</v>
       </c>
@@ -2555,8 +2634,11 @@
       <c r="J24" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>359</v>
       </c>
@@ -2587,8 +2669,11 @@
       <c r="J25" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>360</v>
       </c>
@@ -2619,8 +2704,11 @@
       <c r="J26" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>361</v>
       </c>
@@ -2651,8 +2739,11 @@
       <c r="J27" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>362</v>
       </c>
@@ -2683,8 +2774,11 @@
       <c r="J28" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>363</v>
       </c>
@@ -2715,8 +2809,11 @@
       <c r="J29" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>364</v>
       </c>
@@ -2747,8 +2844,11 @@
       <c r="J30" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>365</v>
       </c>
@@ -2779,8 +2879,11 @@
       <c r="J31" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>366</v>
       </c>
@@ -2811,8 +2914,11 @@
       <c r="J32" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>367</v>
       </c>
@@ -2843,8 +2949,11 @@
       <c r="J33" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>368</v>
       </c>
@@ -2875,8 +2984,11 @@
       <c r="J34" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>369</v>
       </c>
@@ -2907,8 +3019,11 @@
       <c r="J35" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2939,8 +3054,11 @@
       <c r="J36" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>371</v>
       </c>
@@ -2969,8 +3087,11 @@
       <c r="J37" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>372</v>
       </c>
@@ -2999,8 +3120,11 @@
       <c r="J38" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>373</v>
       </c>
@@ -3031,8 +3155,11 @@
       <c r="J39" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>374</v>
       </c>
@@ -3063,8 +3190,11 @@
       <c r="J40" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>375</v>
       </c>
@@ -3095,8 +3225,11 @@
       <c r="J41" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>376</v>
       </c>
@@ -3127,8 +3260,11 @@
       <c r="J42" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>377</v>
       </c>
@@ -3159,8 +3295,11 @@
       <c r="J43" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -3191,8 +3330,11 @@
       <c r="J44" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>379</v>
       </c>
@@ -3223,8 +3365,11 @@
       <c r="J45" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>380</v>
       </c>
@@ -3255,8 +3400,11 @@
       <c r="J46" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>381</v>
       </c>
@@ -3287,8 +3435,11 @@
       <c r="J47" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>382</v>
       </c>
@@ -3319,8 +3470,11 @@
       <c r="J48" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>383</v>
       </c>
@@ -3351,8 +3505,11 @@
       <c r="J49" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>384</v>
       </c>
@@ -3383,8 +3540,11 @@
       <c r="J50" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>385</v>
       </c>
@@ -3415,8 +3575,11 @@
       <c r="J51" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>386</v>
       </c>
@@ -3447,8 +3610,11 @@
       <c r="J52" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -3479,8 +3645,11 @@
       <c r="J53" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>388</v>
       </c>
@@ -3511,8 +3680,11 @@
       <c r="J54" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>389</v>
       </c>
@@ -3543,8 +3715,11 @@
       <c r="J55" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>390</v>
       </c>
@@ -3575,8 +3750,11 @@
       <c r="J56" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>391</v>
       </c>
@@ -3607,8 +3785,11 @@
       <c r="J57" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>392</v>
       </c>
@@ -3639,8 +3820,11 @@
       <c r="J58" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>393</v>
       </c>
@@ -3671,8 +3855,11 @@
       <c r="J59" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>394</v>
       </c>
@@ -3703,8 +3890,11 @@
       <c r="J60" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>395</v>
       </c>
@@ -3735,8 +3925,11 @@
       <c r="J61" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>396</v>
       </c>
@@ -3767,8 +3960,11 @@
       <c r="J62" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>397</v>
       </c>
@@ -3799,8 +3995,11 @@
       <c r="J63" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>398</v>
       </c>
@@ -3831,8 +4030,11 @@
       <c r="J64" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>399</v>
       </c>
@@ -3863,8 +4065,11 @@
       <c r="J65" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>400</v>
       </c>
@@ -3895,8 +4100,11 @@
       <c r="J66" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>401</v>
       </c>
@@ -3927,8 +4135,11 @@
       <c r="J67" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K67" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>402</v>
       </c>
@@ -3959,8 +4170,11 @@
       <c r="J68" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>403</v>
       </c>
@@ -3991,8 +4205,11 @@
       <c r="J69" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K69" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>404</v>
       </c>
@@ -4023,8 +4240,11 @@
       <c r="J70" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K70" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>405</v>
       </c>
@@ -4055,8 +4275,11 @@
       <c r="J71" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K71" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>406</v>
       </c>
@@ -4087,8 +4310,11 @@
       <c r="J72" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K72" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>407</v>
       </c>
@@ -4119,8 +4345,11 @@
       <c r="J73" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K73" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>408</v>
       </c>
@@ -4151,8 +4380,11 @@
       <c r="J74" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -4183,8 +4415,11 @@
       <c r="J75" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K75" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>410</v>
       </c>
@@ -4215,8 +4450,11 @@
       <c r="J76" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K76" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>411</v>
       </c>
@@ -4247,8 +4485,11 @@
       <c r="J77" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K77" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>412</v>
       </c>
@@ -4279,8 +4520,11 @@
       <c r="J78" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>413</v>
       </c>
@@ -4311,8 +4555,11 @@
       <c r="J79" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K79" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>414</v>
       </c>
@@ -4343,8 +4590,11 @@
       <c r="J80" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K80" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>415</v>
       </c>
@@ -4375,8 +4625,11 @@
       <c r="J81" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K81" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>416</v>
       </c>
@@ -4407,8 +4660,11 @@
       <c r="J82" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K82" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>417</v>
       </c>
@@ -4439,8 +4695,11 @@
       <c r="J83" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K83" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>418</v>
       </c>
@@ -4471,8 +4730,11 @@
       <c r="J84" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>419</v>
       </c>
@@ -4503,8 +4765,11 @@
       <c r="J85" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K85" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>420</v>
       </c>
@@ -4532,8 +4797,11 @@
       <c r="J86" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K86" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>421</v>
       </c>
@@ -4564,8 +4832,11 @@
       <c r="J87" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K87" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>422</v>
       </c>
@@ -4596,8 +4867,11 @@
       <c r="J88" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K88" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>423</v>
       </c>
@@ -4628,8 +4902,11 @@
       <c r="J89" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K89" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>424</v>
       </c>
@@ -4660,8 +4937,11 @@
       <c r="J90" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K90" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>425</v>
       </c>
@@ -4692,8 +4972,11 @@
       <c r="J91" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K91" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>426</v>
       </c>
@@ -4724,8 +5007,11 @@
       <c r="J92" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K92" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>427</v>
       </c>
@@ -4756,8 +5042,11 @@
       <c r="J93" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K93" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>428</v>
       </c>
@@ -4788,8 +5077,11 @@
       <c r="J94" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K94" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>429</v>
       </c>
@@ -4820,8 +5112,11 @@
       <c r="J95" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K95" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>430</v>
       </c>
@@ -4852,8 +5147,11 @@
       <c r="J96" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K96" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>431</v>
       </c>
@@ -4884,8 +5182,11 @@
       <c r="J97" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K97" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>432</v>
       </c>
@@ -4916,8 +5217,11 @@
       <c r="J98" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K98" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>433</v>
       </c>
@@ -4948,8 +5252,11 @@
       <c r="J99" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K99" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>434</v>
       </c>
@@ -4980,8 +5287,11 @@
       <c r="J100" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K100" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>435</v>
       </c>
@@ -5012,8 +5322,11 @@
       <c r="J101" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K101" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>436</v>
       </c>
@@ -5044,8 +5357,11 @@
       <c r="J102" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K102" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>437</v>
       </c>
@@ -5076,8 +5392,11 @@
       <c r="J103" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K103" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>438</v>
       </c>
@@ -5108,8 +5427,11 @@
       <c r="J104" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K104" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>439</v>
       </c>
@@ -5140,8 +5462,11 @@
       <c r="J105" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K105" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>440</v>
       </c>
@@ -5172,8 +5497,11 @@
       <c r="J106" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K106" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>441</v>
       </c>
@@ -5204,8 +5532,11 @@
       <c r="J107" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K107" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>442</v>
       </c>
@@ -5236,8 +5567,11 @@
       <c r="J108" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K108" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>443</v>
       </c>
@@ -5268,8 +5602,11 @@
       <c r="J109" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K109" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>444</v>
       </c>
@@ -5300,8 +5637,11 @@
       <c r="J110" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K110" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>445</v>
       </c>
@@ -5332,8 +5672,11 @@
       <c r="J111" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K111" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>446</v>
       </c>
@@ -5364,8 +5707,11 @@
       <c r="J112" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K112" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>447</v>
       </c>
@@ -5396,8 +5742,11 @@
       <c r="J113" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K113" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>448</v>
       </c>
@@ -5428,8 +5777,11 @@
       <c r="J114" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K114" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>449</v>
       </c>
@@ -5460,8 +5812,11 @@
       <c r="J115" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K115" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>450</v>
       </c>
@@ -5492,8 +5847,11 @@
       <c r="J116" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K116" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>451</v>
       </c>
@@ -5524,8 +5882,11 @@
       <c r="J117" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K117" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>452</v>
       </c>
@@ -5556,8 +5917,11 @@
       <c r="J118" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K118" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>453</v>
       </c>
@@ -5588,8 +5952,11 @@
       <c r="J119" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K119" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>454</v>
       </c>
@@ -5619,6 +5986,9 @@
       </c>
       <c r="J120" t="s">
         <v>459</v>
+      </c>
+      <c r="K120" t="s">
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>